<commit_message>
Continued work on estimate sheet
can read excel properties into formulas now
</commit_message>
<xml_diff>
--- a/test-data/repairCosts.xlsx
+++ b/test-data/repairCosts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="116">
   <si>
     <t>costName</t>
   </si>
@@ -340,13 +340,40 @@
   </si>
   <si>
     <t>Demo - dumpster fees - final clean</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Romeo &amp; Juliet</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Shakespeare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num Sold </t>
+  </si>
+  <si>
+    <t>Date Issued</t>
+  </si>
+  <si>
+    <t>Date Issued (Error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8/18/06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,16 +381,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -371,15 +409,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1600,12 +1662,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="1">
+        <v>39815</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>